<commit_message>
integrating data load logic with shiny
</commit_message>
<xml_diff>
--- a/inst/epivis_shiny/data_dictionaries/universal_data_dictionary.xlsx
+++ b/inst/epivis_shiny/data_dictionaries/universal_data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acrisan/Projects/epivis/inst/epivis_shiny/data_dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D327FE-A152-DC4D-A9BE-1E82C93A9D88}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5C096-683D-DF41-9FBE-489C18C0CBFD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="28800" windowHeight="16560" xr2:uid="{B29B066E-24B1-5248-8680-CB28026D9ECA}"/>
+    <workbookView xWindow="1400" yWindow="1900" windowWidth="28800" windowHeight="16560" xr2:uid="{B29B066E-24B1-5248-8680-CB28026D9ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid category type" error="The GenEpi DRIVE application currently only supports the following data types: _x000a__x000a_geography, temporal, or genomic_x000a__x000a_please assign you variable to one of these categories, or, leave it blank" sqref="B1:B1048576" xr:uid="{6C4EF86A-86FF-0E44-B2A2-B60DCB3014BD}">
-      <formula1>"geography,temporal,genomic"</formula1>
+      <formula1>"latitude,longitude,geography,temporal,genomic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>